<commit_message>
Updated Item class to take mulitple sizes.}
</commit_message>
<xml_diff>
--- a/data/Duct Fitting Schedule Low Pressure Insulated Cladded Rect.xlsx
+++ b/data/Duct Fitting Schedule Low Pressure Insulated Cladded Rect.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://zutarilive-my.sharepoint.com/personal/wynand_venter_zutari_com/Documents/RevitHackathon/HVAC/Revit Schedules/HVAC/Seperate/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paul.nel\Documents\repos\HackOne\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_99A4ACBB1CE3F4D020281F60EA8A35AA4ABFD7CA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4C4C533A-4ACF-4CEB-B9E5-2826DD4A0EF3}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{690A4FCC-1685-4511-AB63-A33BADA0CDFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34932" yWindow="432" windowWidth="22836" windowHeight="13200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1548" yWindow="276" windowWidth="21900" windowHeight="13944" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Duct Fitting Schedule Low Press" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -220,9 +219,6 @@
     <t>M_Rectangular Flanged Transition - Length: 600 mm</t>
   </si>
   <si>
-    <t>1070x745-250x200</t>
-  </si>
-  <si>
     <t>5.456 m²</t>
   </si>
   <si>
@@ -411,6 +407,9 @@
   <si>
     <t>LENMED Duct Fitting Schedule Low Pressure 
 Insulated Cladded Rect</t>
+  </si>
+  <si>
+    <t>1600x745-250x200</t>
   </si>
 </sst>
 </file>
@@ -1250,29 +1249,29 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomRight" activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="54" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="36" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -1311,7 +1310,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1328,7 +1327,7 @@
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -1343,7 +1342,7 @@
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
@@ -1372,7 +1371,7 @@
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>18</v>
       </c>
@@ -1395,7 +1394,7 @@
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>19</v>
       </c>
@@ -1434,7 +1433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>19</v>
       </c>
@@ -1473,7 +1472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>19</v>
       </c>
@@ -1512,7 +1511,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>19</v>
       </c>
@@ -1551,7 +1550,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>19</v>
       </c>
@@ -1590,7 +1589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>19</v>
       </c>
@@ -1629,7 +1628,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
@@ -1668,7 +1667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
@@ -1707,7 +1706,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
@@ -1746,7 +1745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>19</v>
       </c>
@@ -1785,7 +1784,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>19</v>
       </c>
@@ -1824,7 +1823,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>19</v>
       </c>
@@ -1863,7 +1862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>19</v>
       </c>
@@ -1902,7 +1901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>19</v>
       </c>
@@ -1941,7 +1940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
@@ -1980,7 +1979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>19</v>
       </c>
@@ -2019,7 +2018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>19</v>
       </c>
@@ -2058,7 +2057,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>53</v>
       </c>
@@ -2095,7 +2094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>53</v>
       </c>
@@ -2132,7 +2131,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>60</v>
       </c>
@@ -2143,13 +2142,13 @@
         <v>15</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>61</v>
+        <v>124</v>
       </c>
       <c r="E25" s="2">
         <v>3</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>17</v>
@@ -2169,7 +2168,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>60</v>
       </c>
@@ -2180,13 +2179,13 @@
         <v>15</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E26" s="2">
         <v>4</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>17</v>
@@ -2204,7 +2203,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>60</v>
       </c>
@@ -2215,13 +2214,13 @@
         <v>15</v>
       </c>
       <c r="D27" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E27" s="2">
+        <v>1</v>
+      </c>
+      <c r="F27" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="E27" s="2">
-        <v>1</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>66</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>17</v>
@@ -2241,7 +2240,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>60</v>
       </c>
@@ -2252,19 +2251,19 @@
         <v>15</v>
       </c>
       <c r="D28" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E28" s="2">
+        <v>1</v>
+      </c>
+      <c r="F28" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E28" s="2">
-        <v>1</v>
-      </c>
-      <c r="F28" s="2" t="s">
+      <c r="G28" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H28" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>69</v>
       </c>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
@@ -2278,7 +2277,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>60</v>
       </c>
@@ -2289,19 +2288,19 @@
         <v>15</v>
       </c>
       <c r="D29" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E29" s="2">
+        <v>1</v>
+      </c>
+      <c r="F29" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E29" s="2">
-        <v>1</v>
-      </c>
-      <c r="F29" s="2" t="s">
+      <c r="G29" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H29" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>72</v>
       </c>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
@@ -2315,7 +2314,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>60</v>
       </c>
@@ -2326,19 +2325,19 @@
         <v>15</v>
       </c>
       <c r="D30" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E30" s="2">
+        <v>1</v>
+      </c>
+      <c r="F30" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="E30" s="2">
-        <v>1</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>74</v>
-      </c>
       <c r="G30" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
@@ -2352,7 +2351,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>60</v>
       </c>
@@ -2363,13 +2362,13 @@
         <v>15</v>
       </c>
       <c r="D31" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E31" s="2">
+        <v>1</v>
+      </c>
+      <c r="F31" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="E31" s="2">
-        <v>1</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>76</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>17</v>
@@ -2389,7 +2388,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>60</v>
       </c>
@@ -2400,13 +2399,13 @@
         <v>15</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E32" s="2">
         <v>2</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>17</v>
@@ -2426,7 +2425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>60</v>
       </c>
@@ -2437,13 +2436,13 @@
         <v>15</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E33" s="2">
         <v>3</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G33" s="2" t="s">
         <v>17</v>
@@ -2463,9 +2462,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -2474,10 +2473,10 @@
         <v>90</v>
       </c>
       <c r="F34" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G34" s="2" t="s">
         <v>82</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>83</v>
       </c>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
@@ -2486,7 +2485,7 @@
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>19</v>
       </c>
@@ -2497,16 +2496,16 @@
         <v>15</v>
       </c>
       <c r="D35" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E35" s="2">
+        <v>1</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G35" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="E35" s="2">
-        <v>1</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>85</v>
       </c>
       <c r="H35" s="2"/>
       <c r="I35" s="2" t="s">
@@ -2525,7 +2524,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>19</v>
       </c>
@@ -2536,16 +2535,16 @@
         <v>15</v>
       </c>
       <c r="D36" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E36" s="2">
+        <v>1</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G36" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="E36" s="2">
-        <v>1</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>87</v>
       </c>
       <c r="H36" s="2"/>
       <c r="I36" s="2" t="s">
@@ -2564,7 +2563,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>19</v>
       </c>
@@ -2575,16 +2574,16 @@
         <v>15</v>
       </c>
       <c r="D37" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E37" s="2">
+        <v>1</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G37" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="E37" s="2">
-        <v>1</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G37" s="2" t="s">
-        <v>89</v>
       </c>
       <c r="H37" s="2"/>
       <c r="I37" s="2" t="s">
@@ -2603,7 +2602,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>19</v>
       </c>
@@ -2614,16 +2613,16 @@
         <v>15</v>
       </c>
       <c r="D38" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E38" s="2">
+        <v>1</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G38" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="E38" s="2">
-        <v>1</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G38" s="2" t="s">
-        <v>91</v>
       </c>
       <c r="H38" s="2"/>
       <c r="I38" s="2" t="s">
@@ -2642,7 +2641,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>19</v>
       </c>
@@ -2653,16 +2652,16 @@
         <v>15</v>
       </c>
       <c r="D39" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E39" s="2">
+        <v>1</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G39" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="E39" s="2">
-        <v>1</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G39" s="2" t="s">
-        <v>93</v>
       </c>
       <c r="H39" s="2"/>
       <c r="I39" s="2" t="s">
@@ -2681,7 +2680,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>19</v>
       </c>
@@ -2692,7 +2691,7 @@
         <v>15</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E40" s="2">
         <v>2</v>
@@ -2701,7 +2700,7 @@
         <v>17</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H40" s="2"/>
       <c r="I40" s="2" t="s">
@@ -2720,7 +2719,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>60</v>
       </c>
@@ -2731,13 +2730,13 @@
         <v>15</v>
       </c>
       <c r="D41" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E41" s="2">
+        <v>1</v>
+      </c>
+      <c r="F41" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="E41" s="2">
-        <v>1</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>97</v>
       </c>
       <c r="G41" s="2" t="s">
         <v>17</v>
@@ -2757,7 +2756,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>60</v>
       </c>
@@ -2768,13 +2767,13 @@
         <v>15</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E42" s="2">
         <v>2</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G42" s="2" t="s">
         <v>17</v>
@@ -2794,7 +2793,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>60</v>
       </c>
@@ -2805,19 +2804,19 @@
         <v>15</v>
       </c>
       <c r="D43" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E43" s="2">
+        <v>1</v>
+      </c>
+      <c r="F43" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="E43" s="2">
-        <v>1</v>
-      </c>
-      <c r="F43" s="2" t="s">
+      <c r="G43" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H43" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="G43" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H43" s="2" t="s">
-        <v>102</v>
       </c>
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
@@ -2831,7 +2830,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>60</v>
       </c>
@@ -2842,19 +2841,19 @@
         <v>15</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E44" s="2">
         <v>1</v>
       </c>
       <c r="F44" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H44" s="2" t="s">
         <v>103</v>
-      </c>
-      <c r="G44" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H44" s="2" t="s">
-        <v>104</v>
       </c>
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
@@ -2868,7 +2867,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>60</v>
       </c>
@@ -2879,13 +2878,13 @@
         <v>15</v>
       </c>
       <c r="D45" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E45" s="2">
+        <v>1</v>
+      </c>
+      <c r="F45" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="E45" s="2">
-        <v>1</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>106</v>
       </c>
       <c r="G45" s="2" t="s">
         <v>17</v>
@@ -2905,7 +2904,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>60</v>
       </c>
@@ -2916,13 +2915,13 @@
         <v>15</v>
       </c>
       <c r="D46" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E46" s="2">
+        <v>1</v>
+      </c>
+      <c r="F46" s="2" t="s">
         <v>107</v>
-      </c>
-      <c r="E46" s="2">
-        <v>1</v>
-      </c>
-      <c r="F46" s="2" t="s">
-        <v>108</v>
       </c>
       <c r="G46" s="2" t="s">
         <v>17</v>
@@ -2942,7 +2941,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>60</v>
       </c>
@@ -2953,13 +2952,13 @@
         <v>15</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E47" s="2">
         <v>2</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G47" s="2" t="s">
         <v>17</v>
@@ -2979,7 +2978,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>60</v>
       </c>
@@ -2990,19 +2989,19 @@
         <v>15</v>
       </c>
       <c r="D48" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E48" s="2">
+        <v>1</v>
+      </c>
+      <c r="F48" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="E48" s="2">
-        <v>1</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>112</v>
-      </c>
       <c r="G48" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
@@ -3016,7 +3015,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>60</v>
       </c>
@@ -3027,13 +3026,13 @@
         <v>15</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E49" s="2">
         <v>4</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G49" s="2" t="s">
         <v>17</v>
@@ -3053,9 +3052,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -3064,10 +3063,10 @@
         <v>21</v>
       </c>
       <c r="F50" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="G50" s="2" t="s">
         <v>116</v>
-      </c>
-      <c r="G50" s="2" t="s">
-        <v>117</v>
       </c>
       <c r="H50" s="2"/>
       <c r="I50" s="2"/>
@@ -3076,7 +3075,7 @@
       <c r="L50" s="2"/>
       <c r="M50" s="2"/>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>19</v>
       </c>
@@ -3087,7 +3086,7 @@
         <v>15</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E51" s="2">
         <v>4</v>
@@ -3096,7 +3095,7 @@
         <v>17</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H51" s="2"/>
       <c r="I51" s="2" t="s">
@@ -3115,7 +3114,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>60</v>
       </c>
@@ -3126,13 +3125,13 @@
         <v>15</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E52" s="2">
         <v>2</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G52" s="2" t="s">
         <v>17</v>
@@ -3152,9 +3151,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
@@ -3163,10 +3162,10 @@
         <v>6</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H53" s="2"/>
       <c r="I53" s="2"/>
@@ -3175,9 +3174,9 @@
       <c r="L53" s="2"/>
       <c r="M53" s="2"/>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
@@ -3186,10 +3185,10 @@
         <v>118</v>
       </c>
       <c r="F54" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="G54" s="2" t="s">
         <v>122</v>
-      </c>
-      <c r="G54" s="2" t="s">
-        <v>123</v>
       </c>
       <c r="H54" s="2"/>
       <c r="I54" s="2"/>

</xml_diff>